<commit_message>
changing benthic chlorophyl sheet
</commit_message>
<xml_diff>
--- a/Benthic_Chlorophyll.xlsx
+++ b/Benthic_Chlorophyll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviaaguiar/Desktop/LUMCON REU/Project/LUMCONREU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA5F370-FD82-8548-95BF-01B46851CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8956D01-BD53-3E4E-89BA-2D000E52B061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,32 +95,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <r>
-      <t>Chl a                    (mg cm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -257,6 +231,9 @@
   </si>
   <si>
     <t>Latitude (decimal degrees)</t>
+  </si>
+  <si>
+    <t>Chl_a</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1296,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1355,10 +1332,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>4</v>
@@ -1367,22 +1344,22 @@
         <v>5</v>
       </c>
       <c r="I1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="22" t="s">
         <v>29</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>